<commit_message>
Limbs rewrite + start of coding
1/2 of limbs fixed,
barebones of python script
</commit_message>
<xml_diff>
--- a/Limbs.xlsx
+++ b/Limbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kage\Documents\GitHub\Sculpt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5D9DDC-30E4-4A2A-9414-A731C0B8AAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A06ADC-5CF1-4F89-9338-DA063114CD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="129">
   <si>
     <t>Name</t>
   </si>
@@ -81,9 +81,6 @@
     <t>&lt;b&gt;Rancor: &lt;/b&gt;2 AP + weirdTJazzT&lt;br&gt;Mark a target as your hated target. You can only have one target at a time.</t>
   </si>
   <si>
-    <t>&lt;i&gt;Ranged Attack -&lt;/i&gt;&lt;b&gt; Scorn:&lt;/b&gt; 2 AP&lt;br&gt;This attack can only hit your hated target&lt;br&gt;Damage = 4&lt;br&gt;Crit option&lt;br&gt;&lt;b&gt;Omen:&lt;/b&gt; inflict the &lt;b&gt;Cursed&lt;/b&gt; status effect</t>
-  </si>
-  <si>
     <t>Bladed Fingers</t>
   </si>
   <si>
@@ -108,12 +105,6 @@
     <t>Cicada Wings</t>
   </si>
   <si>
-    <t>&lt;b&gt;Fly: &lt;/b&gt;1 AP or  weirdT&lt;br&gt;Make a move action with + 1 speed, ignore terrain during this move (within reason).</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Chirp Tune: &lt;/b&gt;2 AP&lt;br&gt;You and any number of target allies each gain up to 3 temporary composure.</t>
-  </si>
-  <si>
     <t>Clay Exuder</t>
   </si>
   <si>
@@ -126,18 +117,9 @@
     <t>Clayling</t>
   </si>
   <si>
-    <t>&lt;i&gt;Passive -&lt;b&gt; Autonomous Limb: &lt;/i&gt;&lt;/b&gt;&lt;br&gt;At the end of your turn, this limb makes an attack for free, it will attack you if there are no other targets available.</t>
-  </si>
-  <si>
-    <t>&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Flail:&lt;/b&gt;&lt;br&gt;Damage = 4 , close range.</t>
-  </si>
-  <si>
     <t>Crackling Geode</t>
   </si>
   <si>
-    <t>Whenever you spend weirdt, deal 1 damage to any target. This damage cannot be reduced.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;span style="color:#27ae60"&gt;&lt;strong&gt;Jazz&lt;/strong&gt;&lt;/span&gt;</t>
   </si>
   <si>
@@ -159,9 +141,6 @@
     <t>&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Thwack: &lt;/b&gt;1 AP&lt;br&gt;Damage = 1 , close range.&lt;br&gt;Critical Options:&lt;br&gt;&lt;b&gt;Omen:&lt;/b&gt; Inflict the &lt;b&gt;Cursed&lt;/b&gt; status effect.</t>
   </si>
   <si>
-    <t>&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Block:&lt;/b&gt; 1 AP&lt;br&gt;Destroy this card to completely block an incoming attack.</t>
-  </si>
-  <si>
     <t>&lt;span style="color:#3366cc"&gt;&lt;strong&gt;Weird&lt;/strong&gt;&lt;/span&gt;</t>
   </si>
   <si>
@@ -177,27 +156,18 @@
     <t>Granite Fists</t>
   </si>
   <si>
-    <t>&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Crush:&lt;/b&gt; 4 AP or (2 AP + fleshTfleshT)&lt;br&gt;Damage = 8 , close range.&lt;br&gt;Critical Options:&lt;b&gt;&lt;br&gt;Concuss:&lt;/b&gt; Inflict the &lt;b&gt;Stunned&lt;/b&gt; status effect.</t>
-  </si>
-  <si>
     <t>Grasp of Mud</t>
   </si>
   <si>
     <t>&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Bludgeon:&lt;/b&gt; 3 AP&lt;br&gt;Damage = 6 , close range.</t>
   </si>
   <si>
-    <t>&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Whelm:&lt;/b&gt; 2 AP + weirdT&lt;br&gt;Damage = 3 , close range.&lt;br&gt;Inflicts the &lt;b&gt;Entangled&lt;/b&gt; status effect on a hit.</t>
-  </si>
-  <si>
     <t>Horns</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
-    <t>&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Charge!:&lt;/b&gt; 3 AP or 2 AP +jazzT&lt;br&gt;Damage = hexes moved , close range.&lt;br&gt;You may move any number of hexes in a straight line as part of making the attack. &lt;br&gt;hornshexes</t>
-  </si>
-  <si>
     <t>&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Shove :&lt;/b&gt; 1 AP +fleshT&lt;br&gt;Damage = 2 , close range.&lt;br&gt;On a hit, the target is pushed back hexes equal to your &lt;span style="color:#e74c3c"&gt;&lt;strong&gt;Flesh&lt;/strong&gt;&lt;/span&gt;.</t>
   </si>
   <si>
@@ -207,30 +177,15 @@
     <t>&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Nip:&lt;/b&gt; 2 AP&lt;br&gt;Damage = &lt;span style="color:#e74c3c"&gt;&lt;strong&gt;Flesh&lt;/strong&gt;&lt;/span&gt; , close range.&lt;br&gt;Critical Option:&lt;br&gt;&lt;b&gt;Restrain: &lt;/b&gt;Inflict the &lt;b&gt;Entangled&lt;/b&gt; status effect.</t>
   </si>
   <si>
-    <t>&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Block: &lt;/b&gt;1 AP&lt;br&gt;Destroy this card to completely block an incoming attack.</t>
-  </si>
-  <si>
     <t>Hungering Hand</t>
   </si>
   <si>
-    <t>&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Bite:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 4 , close range.&lt;br&gt;Critical Option:&lt;br&gt;&lt;b&gt;Exalt:&lt;/b&gt; Restore your composure or gain up to 2 temporary composure.</t>
-  </si>
-  <si>
     <t>&lt;i&gt;Ranged Attack -&lt;/i&gt;&lt;b&gt; Phage: &lt;/b&gt;2 AP&lt;br&gt;Damage = 7 &lt;br&gt;Throw this limb at your target as part of the attack, regardless of attack outcome, they now have Hungering Hand equipped .</t>
   </si>
   <si>
     <t>Lanceflower Bloom</t>
   </si>
   <si>
-    <t>&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Impale: &lt;/b&gt;2 AP&lt;br&gt;Damage = 5 , reach.&lt;br&gt;Must be in lance mode to use.</t>
-  </si>
-  <si>
-    <t>&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Iron Petals: &lt;/b&gt;1 AP&lt;br&gt;Destroy this card to completely block an incoming attack.&lt;br&gt;Must be in flower mode to use.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Bloom/Wither:&lt;/b&gt; 1 AP&lt;br&gt;Switch this card between lance mode or Flower mode. At the start of the combat Lanceflower Bloom begins in Flower mode.</t>
-  </si>
-  <si>
     <t>Lithium Geode</t>
   </si>
   <si>
@@ -406,6 +361,72 @@
   </si>
   <si>
     <t>Explosive Lesion</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Ranged Attack -&lt;/i&gt;&lt;b&gt; Scorn:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 4&lt;br&gt;This attack can only target your hated target.&lt;br&gt;Critical options:&lt;br&gt;&lt;b&gt;Omen:&lt;/b&gt; inflict the &lt;b&gt;Cursed&lt;/b&gt; status effect</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Fly: &lt;/b&gt;2 AP or  weirdT&lt;br&gt;Make a move action with + 1 speed, ignore terrain during this move (within reason).</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Chirp Tune: &lt;/b&gt;3 AP&lt;br&gt;You and any number of target allies each gain up to 3 temporary composure.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Passive -&lt;b&gt; Autonomous Limb: &lt;/i&gt;&lt;/b&gt;&lt;br&gt;At the end of your turn, this limb uses &lt;b&gt;Flail&lt;/b&gt; for free, it will target you if there are no other targets available.&lt;br&gt;Melee Attack - &lt;b&gt;Flail:&lt;br&gt;&lt;/b&gt;Damage = 4, close range.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Back-kick: &lt;/b&gt;2 AP&lt;br&gt;Damage = 4 , close range.&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>Critical options:&lt;br&gt;&lt;b&gt;Dash:&lt;/b&gt; Take a move action.&lt;br&gt;&lt;b&gt;Mighty Shove:&lt;/b&gt; Push the target 2 hexes.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Shock: &lt;/b&gt;2 AP&lt;br&gt;Damage = 1 , reach.&lt;br&gt;This damage cannot be reduced.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Smash: &lt;/b&gt;2 AP + 3 Composure&lt;br&gt;Damage = 5 , close range.&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Drive-Power: &lt;/b&gt;weirdt&lt;br&gt;Add +1 damage and +1 range to attacks this turn, use only once each turn.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Smear:&lt;/b&gt; 2 AP + weirdT weirdT&lt;br&gt;Inflict the &lt;b&gt;Cursed&lt;/b&gt; status effect on a target in close range.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Burst Block: &lt;/b&gt;&lt;br&gt;Destroy this card to completely block an incoming attack and deal 5 damage to all adjacent beings.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Lay Egg:&lt;/b&gt; 1 AP + (chargeT or  weirdT)&lt;br&gt;Place an explosive egg on an adjacent hex.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Detonate:&lt;/b&gt; 1 AP&lt;br&gt;All eggs on the map explode, adjacent beings take 5 damage and terrain is destroyed, including walls.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Whelm:&lt;/b&gt; 1 AP + weirdT&lt;br&gt;Damage = 3 , close range.&lt;br&gt;Inflicts the &lt;b&gt;Entangled&lt;/b&gt; status effect on a hit.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Passive -&lt;b&gt; Sparks: &lt;/i&gt;&lt;/b&gt;Whenever you spend weirdt, deal 1 damage to any target. This damage cannot be reduced.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Vandalise:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 2 , close range.&lt;br&gt;On a hit, you may destroy this card to destroy any equipped Limb or Impression from the target.</t>
+  </si>
+  <si>
+    <t>chargeBIG chargeBIG</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Crush:&lt;/b&gt; 4 AP or (2 AP + fleshT fleshT)&lt;br&gt;Damage = 8 , close range.&lt;br&gt;Critical Options:&lt;b&gt;&lt;br&gt;Concuss:&lt;/b&gt; Inflict the &lt;b&gt;Stunned&lt;/b&gt; status effect.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Charge!:&lt;/b&gt; 2 AP&lt;br&gt;Damage = hexes moved , close range.&lt;br&gt;You may move any number of hexes in a straight line as part of making the attack. &lt;br&gt;hornshexes</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Bite:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 4 , close range.&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Impale: &lt;/b&gt;2 AP&lt;br&gt;Damage = 4 , reach.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Bloom: &lt;/b&gt; WeirdT + &lt;b&gt;exhausted&lt;/b&gt; &lt;br&gt;Destroy this card to completely block an incoming attack.</t>
   </si>
 </sst>
 </file>
@@ -510,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -534,10 +555,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -545,427 +565,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6B0DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6B0DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6B0DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6B0DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6B0DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6B0DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6B0DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6B0DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6B0DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6B0DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6B0DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6B0DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -1280,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1344,16 +944,19 @@
         <v>12</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="7"/>
+      <c r="J2" s="7" t="str">
+        <f>IF(C2="yes",_xlfn.CONCAT($N$3,E2,IF(F2="","","&lt;img src=images\inline\linebrk.png&gt;"),F2,IF(G2="","","&lt;img src=images\inline\linebrk.png&gt;"),G2,IF(H2="","","&lt;img src=images\inline\linebrk.png&gt;"),H2,),_xlfn.CONCAT($M$3,E2,IF(F2="","","&lt;img src=images\inline\linebrk.png&gt;"),F2,IF(G2="","","&lt;img src=images\inline\linebrk.png&gt;"),G2,IF(H2="","","&lt;img src=images\inline\linebrk.png&gt;"),H2,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Rancor: &lt;/b&gt;2 AP + weirdTJazzT&lt;br&gt;Mark a target as your hated target. You can only have one target at a time.&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Ranged Attack -&lt;/i&gt;&lt;b&gt; Scorn:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 4&lt;br&gt;This attack can only target your hated target.&lt;br&gt;Critical options:&lt;br&gt;&lt;b&gt;Omen:&lt;/b&gt; inflict the &lt;b&gt;Cursed&lt;/b&gt; status effect</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>11</v>
@@ -1361,26 +964,26 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7" t="str">
-        <f>IF(C3="yes",_xlfn.CONCAT($N$3,E3,IF(F3="","","&lt;img src=Images\line.png&gt;"),F3,IF(G3="","","&lt;img src=Images\line.png&gt;"),G3,IF(H3="","","&lt;img src=Images\line.png&gt;"),H3,),_xlfn.CONCAT($M$3,E3,IF(F3="","","&lt;img src=Images\line.png&gt;"),F3,IF(G3="","","&lt;img src=Images\line.png&gt;"),G3,IF(H3="","","&lt;img src=Images\line.png&gt;"),H3,))</f>
+        <f>IF(C3="yes",_xlfn.CONCAT($N$3,E3,IF(F3="","","&lt;img src=images\inline\linebrk.png&gt;"),F3,IF(G3="","","&lt;img src=images\inline\linebrk.png&gt;"),G3,IF(H3="","","&lt;img src=images\inline\linebrk.png&gt;"),H3,),_xlfn.CONCAT($M$3,E3,IF(F3="","","&lt;img src=images\inline\linebrk.png&gt;"),F3,IF(G3="","","&lt;img src=images\inline\linebrk.png&gt;"),G3,IF(H3="","","&lt;img src=images\inline\linebrk.png&gt;"),H3,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; 1000 Cuts: &lt;/b&gt;2 AP&lt;br&gt;Damage = 3 , close range.&lt;br&gt;Critical options:&lt;br&gt;&lt;b&gt;Flurry:&lt;/b&gt;Your next attack costs 1 less AP.&lt;br&gt;&lt;b&gt;Strike:&lt;/b&gt; +1 Damage.</v>
       </c>
       <c r="M3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" t="s">
         <v>16</v>
-      </c>
-      <c r="N3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>11</v>
@@ -1388,19 +991,22 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="7"/>
+      <c r="J4" s="7" t="str">
+        <f>IF(C4="yes",_xlfn.CONCAT($N$3,E4,IF(F4="","","&lt;img src=images\inline\linebrk.png&gt;"),F4,IF(G4="","","&lt;img src=images\inline\linebrk.png&gt;"),G4,IF(H4="","","&lt;img src=images\inline\linebrk.png&gt;"),H4,),_xlfn.CONCAT($M$3,E4,IF(F4="","","&lt;img src=images\inline\linebrk.png&gt;"),F4,IF(G4="","","&lt;img src=images\inline\linebrk.png&gt;"),G4,IF(H4="","","&lt;img src=images\inline\linebrk.png&gt;"),H4,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Create Sigil: &lt;/b&gt;1 AP&lt;br&gt;Draw a sigil on an adjacent tile. You may have a maximum of 3 sigils. Creating more will destroy a sigil of your choice. Other players may spend 3AP to destroy an adjacent sigil&lt;img src=images\inline\linebrk.png&gt;&lt;b&gt;Siphon: &lt;/b&gt;2 AP + weirdT&lt;br&gt;If there are 3 sigils, deal a random wound to all creatures within the triangle of sigils (edges count). Heal a wound of your choice.</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>11</v>
@@ -1408,22 +1014,22 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>22</v>
+        <v>108</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7" t="str">
-        <f>IF(C5="yes",_xlfn.CONCAT($N$3,E5,IF(F5="","","&lt;img src=Images\line.png&gt;"),F5,IF(G5="","","&lt;img src=Images\line.png&gt;"),G5,IF(H5="","","&lt;img src=Images\line.png&gt;"),H5,),_xlfn.CONCAT($M$3,E5,IF(F5="","","&lt;img src=Images\line.png&gt;"),F5,IF(G5="","","&lt;img src=Images\line.png&gt;"),G5,IF(H5="","","&lt;img src=Images\line.png&gt;"),H5,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Fly: &lt;/b&gt;1 AP or  weirdT&lt;br&gt;Make a move action with + 1 speed, ignore terrain during this move (within reason).&lt;img src=Images\line.png&gt;&lt;b&gt;Chirp Tune: &lt;/b&gt;2 AP&lt;br&gt;You and any number of target allies each gain up to 3 temporary composure.</v>
+        <f>IF(C5="yes",_xlfn.CONCAT($N$3,E5,IF(F5="","","&lt;img src=images\inline\linebrk.png&gt;"),F5,IF(G5="","","&lt;img src=images\inline\linebrk.png&gt;"),G5,IF(H5="","","&lt;img src=images\inline\linebrk.png&gt;"),H5,),_xlfn.CONCAT($M$3,E5,IF(F5="","","&lt;img src=images\inline\linebrk.png&gt;"),F5,IF(G5="","","&lt;img src=images\inline\linebrk.png&gt;"),G5,IF(H5="","","&lt;img src=images\inline\linebrk.png&gt;"),H5,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Fly: &lt;/b&gt;2 AP or  weirdT&lt;br&gt;Make a move action with + 1 speed, ignore terrain during this move (within reason).&lt;img src=images\inline\linebrk.png&gt;&lt;b&gt;Chirp Tune: &lt;/b&gt;3 AP&lt;br&gt;You and any number of target allies each gain up to 3 temporary composure.</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>11</v>
@@ -1431,22 +1037,22 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="7" t="str">
-        <f>IF(C6="yes",_xlfn.CONCAT($N$3,E6,IF(F6="","","&lt;img src=Images\line.png&gt;"),F6,IF(G6="","","&lt;img src=Images\line.png&gt;"),G6,IF(H6="","","&lt;img src=Images\line.png&gt;"),H6,),_xlfn.CONCAT($M$3,E6,IF(F6="","","&lt;img src=Images\line.png&gt;"),F6,IF(G6="","","&lt;img src=Images\line.png&gt;"),G6,IF(H6="","","&lt;img src=Images\line.png&gt;"),H6,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Coat in Clay: &lt;/b&gt;1 AP +  weirdT&lt;br&gt;A target gains up to 4 temporary composure and -2 speed until the end of their next turn.&lt;img src=Images\line.png&gt;&lt;i&gt;Passive -&lt;b&gt; Spreading clay: &lt;/i&gt;&lt;/b&gt;&lt;br&gt;Whenever you spend weirdt, gain up to 1 temporary composure.</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+        <f>IF(C6="yes",_xlfn.CONCAT($N$3,E6,IF(F6="","","&lt;img src=images\inline\linebrk.png&gt;"),F6,IF(G6="","","&lt;img src=images\inline\linebrk.png&gt;"),G6,IF(H6="","","&lt;img src=images\inline\linebrk.png&gt;"),H6,),_xlfn.CONCAT($M$3,E6,IF(F6="","","&lt;img src=images\inline\linebrk.png&gt;"),F6,IF(G6="","","&lt;img src=images\inline\linebrk.png&gt;"),G6,IF(H6="","","&lt;img src=images\inline\linebrk.png&gt;"),H6,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Coat in Clay: &lt;/b&gt;1 AP +  weirdT&lt;br&gt;A target gains up to 4 temporary composure and -2 speed until the end of their next turn.&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Passive -&lt;b&gt; Spreading clay: &lt;/i&gt;&lt;/b&gt;&lt;br&gt;Whenever you spend weirdt, gain up to 1 temporary composure.</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>11</v>
@@ -1454,68 +1060,75 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>29</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="7" t="str">
-        <f>IF(C7="yes",_xlfn.CONCAT($N$3,E7,IF(F7="","","&lt;img src=Images\line.png&gt;"),F7,IF(G7="","","&lt;img src=Images\line.png&gt;"),G7,IF(H7="","","&lt;img src=Images\line.png&gt;"),H7,),_xlfn.CONCAT($M$3,E7,IF(F7="","","&lt;img src=Images\line.png&gt;"),F7,IF(G7="","","&lt;img src=Images\line.png&gt;"),G7,IF(H7="","","&lt;img src=Images\line.png&gt;"),H7,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Passive -&lt;b&gt; Autonomous Limb: &lt;/i&gt;&lt;/b&gt;&lt;br&gt;At the end of your turn, this limb makes an attack for free, it will attack you if there are no other targets available.&lt;img src=Images\line.png&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Flail:&lt;/b&gt;&lt;br&gt;Damage = 4 , close range.</v>
+        <f>IF(C7="yes",_xlfn.CONCAT($N$3,E7,IF(F7="","","&lt;img src=images\inline\linebrk.png&gt;"),F7,IF(G7="","","&lt;img src=images\inline\linebrk.png&gt;"),G7,IF(H7="","","&lt;img src=images\inline\linebrk.png&gt;"),H7,),_xlfn.CONCAT($M$3,E7,IF(F7="","","&lt;img src=images\inline\linebrk.png&gt;"),F7,IF(G7="","","&lt;img src=images\inline\linebrk.png&gt;"),G7,IF(H7="","","&lt;img src=images\inline\linebrk.png&gt;"),H7,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Passive -&lt;b&gt; Autonomous Limb: &lt;/i&gt;&lt;/b&gt;&lt;br&gt;At the end of your turn, this limb uses &lt;b&gt;Flail&lt;/b&gt; for free, it will target you if there are no other targets available.&lt;br&gt;Melee Attack - &lt;b&gt;Flail:&lt;br&gt;&lt;/b&gt;Damage = 4, close range.</v>
       </c>
       <c r="K7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>112</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="7"/>
+      <c r="J8" s="7" t="str">
+        <f>IF(C8="yes",_xlfn.CONCAT($N$3,E8,IF(F8="","","&lt;img src=images\inline\linebrk.png&gt;"),F8,IF(G8="","","&lt;img src=images\inline\linebrk.png&gt;"),G8,IF(H8="","","&lt;img src=images\inline\linebrk.png&gt;"),H8,),_xlfn.CONCAT($M$3,E8,IF(F8="","","&lt;img src=images\inline\linebrk.png&gt;"),F8,IF(G8="","","&lt;img src=images\inline\linebrk.png&gt;"),G8,IF(H8="","","&lt;img src=images\inline\linebrk.png&gt;"),H8,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Back-kick: &lt;/b&gt;2 AP&lt;br&gt;Damage = 4 , close range.&lt;br&gt;&lt;img src=images\inline\linebrk.png&gt;Critical options:&lt;br&gt;&lt;b&gt;Dash:&lt;/b&gt; Take a move action.&lt;br&gt;&lt;b&gt;Mighty Shove:&lt;/b&gt; Push the target 2 hexes.</v>
+      </c>
       <c r="K8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="6"/>
+      <c r="E9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>121</v>
+      </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="7" t="str">
-        <f>IF(C9="yes",_xlfn.CONCAT($N$3,E9,IF(F9="","","&lt;img src=Images\line.png&gt;"),F9,IF(G9="","","&lt;img src=Images\line.png&gt;"),G9,IF(H9="","","&lt;img src=Images\line.png&gt;"),H9,),_xlfn.CONCAT($M$3,E9,IF(F9="","","&lt;img src=Images\line.png&gt;"),F9,IF(G9="","","&lt;img src=Images\line.png&gt;"),G9,IF(H9="","","&lt;img src=Images\line.png&gt;"),H9,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;Whenever you spend weirdt, deal 1 damage to any target. This damage cannot be reduced.</v>
+        <f>IF(C9="yes",_xlfn.CONCAT($N$3,E9,IF(F9="","","&lt;img src=images\inline\linebrk.png&gt;"),F9,IF(G9="","","&lt;img src=images\inline\linebrk.png&gt;"),G9,IF(H9="","","&lt;img src=images\inline\linebrk.png&gt;"),H9,),_xlfn.CONCAT($M$3,E9,IF(F9="","","&lt;img src=images\inline\linebrk.png&gt;"),F9,IF(G9="","","&lt;img src=images\inline\linebrk.png&gt;"),G9,IF(H9="","","&lt;img src=images\inline\linebrk.png&gt;"),H9,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Shock: &lt;/b&gt;2 AP&lt;br&gt;Damage = 1 , reach.&lt;br&gt;This damage cannot be reduced.&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Passive -&lt;b&gt; Sparks: &lt;/i&gt;&lt;/b&gt;Whenever you spend weirdt, deal 1 damage to any target. This damage cannot be reduced.</v>
       </c>
       <c r="K9" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>11</v>
@@ -1523,38 +1136,45 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="7" t="str">
-        <f>IF(C10="yes",_xlfn.CONCAT($N$3,E10,IF(F10="","","&lt;img src=Images\line.png&gt;"),F10,IF(G10="","","&lt;img src=Images\line.png&gt;"),G10,IF(H10="","","&lt;img src=Images\line.png&gt;"),H10,),_xlfn.CONCAT($M$3,E10,IF(F10="","","&lt;img src=Images\line.png&gt;"),F10,IF(G10="","","&lt;img src=Images\line.png&gt;"),G10,IF(H10="","","&lt;img src=Images\line.png&gt;"),H10,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Embed: &lt;/b&gt;weirdT&lt;br&gt;Place a 1 hex crystal on an adjacent hex. The crystal breaks if it takes damage.&lt;img src=Images\line.png&gt;&lt;i&gt;Passive -&lt;b&gt; Radiance: &lt;/b&gt;&lt;/i&gt;&lt;br&gt;At the end of your turn, if you are adjacent to a crystal, choose one of the following status effects to gain:&lt;br&gt;&lt;b&gt;Monstrous, Well Rested, Imbued.</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <f>IF(C10="yes",_xlfn.CONCAT($N$3,E10,IF(F10="","","&lt;img src=images\inline\linebrk.png&gt;"),F10,IF(G10="","","&lt;img src=images\inline\linebrk.png&gt;"),G10,IF(H10="","","&lt;img src=images\inline\linebrk.png&gt;"),H10,),_xlfn.CONCAT($M$3,E10,IF(F10="","","&lt;img src=images\inline\linebrk.png&gt;"),F10,IF(G10="","","&lt;img src=images\inline\linebrk.png&gt;"),G10,IF(H10="","","&lt;img src=images\inline\linebrk.png&gt;"),H10,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Embed: &lt;/b&gt;weirdT&lt;br&gt;Place a 1 hex crystal on an adjacent hex. The crystal breaks if it takes damage.&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Passive -&lt;b&gt; Radiance: &lt;/b&gt;&lt;/i&gt;&lt;br&gt;At the end of your turn, if you are adjacent to a crystal, choose one of the following status effects to gain:&lt;br&gt;&lt;b&gt;Monstrous, Well Rested, Imbued.</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="J11" s="7" t="str">
+        <f>IF(C11="yes",_xlfn.CONCAT($N$3,E11,IF(F11="","","&lt;img src=images\inline\linebrk.png&gt;"),F11,IF(G11="","","&lt;img src=images\inline\linebrk.png&gt;"),G11,IF(H11="","","&lt;img src=images\inline\linebrk.png&gt;"),H11,),_xlfn.CONCAT($M$3,E11,IF(F11="","","&lt;img src=images\inline\linebrk.png&gt;"),F11,IF(G11="","","&lt;img src=images\inline\linebrk.png&gt;"),G11,IF(H11="","","&lt;img src=images\inline\linebrk.png&gt;"),H11,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Smash: &lt;/b&gt;2 AP + 3 Composure&lt;br&gt;Damage = 5 , close range.&lt;br&gt;&lt;img src=images\inline\linebrk.png&gt;&lt;b&gt;Drive-Power: &lt;/b&gt;weirdt&lt;br&gt;Add +1 damage and +1 range to attacks this turn, use only once each turn.</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>11</v>
@@ -1562,22 +1182,22 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="7" t="str">
-        <f>IF(C12="yes",_xlfn.CONCAT($N$3,E12,IF(F12="","","&lt;img src=Images\line.png&gt;"),F12,IF(G12="","","&lt;img src=Images\line.png&gt;"),G12,IF(H12="","","&lt;img src=Images\line.png&gt;"),H12,),_xlfn.CONCAT($M$3,E12,IF(F12="","","&lt;img src=Images\line.png&gt;"),F12,IF(G12="","","&lt;img src=Images\line.png&gt;"),G12,IF(H12="","","&lt;img src=Images\line.png&gt;"),H12,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Thwack: &lt;/b&gt;1 AP&lt;br&gt;Damage = 1 , close range.&lt;br&gt;Critical Options:&lt;br&gt;&lt;b&gt;Omen:&lt;/b&gt; Inflict the &lt;b&gt;Cursed&lt;/b&gt; status effect.&lt;img src=Images\line.png&gt;&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Block:&lt;/b&gt; 1 AP&lt;br&gt;Destroy this card to completely block an incoming attack.</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+        <f>IF(C12="yes",_xlfn.CONCAT($N$3,E12,IF(F12="","","&lt;img src=images\inline\linebrk.png&gt;"),F12,IF(G12="","","&lt;img src=images\inline\linebrk.png&gt;"),G12,IF(H12="","","&lt;img src=images\inline\linebrk.png&gt;"),H12,),_xlfn.CONCAT($M$3,E12,IF(F12="","","&lt;img src=images\inline\linebrk.png&gt;"),F12,IF(G12="","","&lt;img src=images\inline\linebrk.png&gt;"),G12,IF(H12="","","&lt;img src=images\inline\linebrk.png&gt;"),H12,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Thwack: &lt;/b&gt;1 AP&lt;br&gt;Damage = 1 , close range.&lt;br&gt;Critical Options:&lt;br&gt;&lt;b&gt;Omen:&lt;/b&gt; Inflict the &lt;b&gt;Cursed&lt;/b&gt; status effect.&lt;img src=images\inline\linebrk.png&gt;&lt;b&gt;Smear:&lt;/b&gt; 2 AP + weirdT weirdT&lt;br&gt;Inflict the &lt;b&gt;Cursed&lt;/b&gt; status effect on a target in close range.</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>11</v>
@@ -1585,54 +1205,67 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="7" t="str">
-        <f>IF(C13="yes",_xlfn.CONCAT($N$3,E13,IF(F13="","","&lt;img src=Images\line.png&gt;"),F13,IF(G13="","","&lt;img src=Images\line.png&gt;"),G13,IF(H13="","","&lt;img src=Images\line.png&gt;"),H13,),_xlfn.CONCAT($M$3,E13,IF(F13="","","&lt;img src=Images\line.png&gt;"),F13,IF(G13="","","&lt;img src=Images\line.png&gt;"),G13,IF(H13="","","&lt;img src=Images\line.png&gt;"),H13,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt; &lt;b&gt;Flay:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 3 , close range.&lt;br&gt;Critical Options:&lt;br&gt;&lt;b&gt;Burn:&lt;/b&gt; Inflict the &lt;b&gt;Burning&lt;/b&gt; status effect.&lt;img src=Images\line.png&gt;&lt;b&gt;Stoke the Flames:&lt;/b&gt; WeirdT&lt;br&gt;Your attacks this turn inflict the &lt;b&gt;Burning&lt;/b&gt; status effect on a hit and have + 1 range</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <f>IF(C13="yes",_xlfn.CONCAT($N$3,E13,IF(F13="","","&lt;img src=images\inline\linebrk.png&gt;"),F13,IF(G13="","","&lt;img src=images\inline\linebrk.png&gt;"),G13,IF(H13="","","&lt;img src=images\inline\linebrk.png&gt;"),H13,),_xlfn.CONCAT($M$3,E13,IF(F13="","","&lt;img src=images\inline\linebrk.png&gt;"),F13,IF(G13="","","&lt;img src=images\inline\linebrk.png&gt;"),G13,IF(H13="","","&lt;img src=images\inline\linebrk.png&gt;"),H13,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt; &lt;b&gt;Flay:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 3 , close range.&lt;br&gt;Critical Options:&lt;br&gt;&lt;b&gt;Burn:&lt;/b&gt; Inflict the &lt;b&gt;Burning&lt;/b&gt; status effect.&lt;img src=images\inline\linebrk.png&gt;&lt;b&gt;Stoke the Flames:&lt;/b&gt; WeirdT&lt;br&gt;Your attacks this turn inflict the &lt;b&gt;Burning&lt;/b&gt; status effect on a hit and have + 1 range</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="J14" s="7" t="str">
+        <f>IF(C14="yes",_xlfn.CONCAT($N$3,E14,IF(F14="","","&lt;img src=images\inline\linebrk.png&gt;"),F14,IF(G14="","","&lt;img src=images\inline\linebrk.png&gt;"),G14,IF(H14="","","&lt;img src=images\inline\linebrk.png&gt;"),H14,),_xlfn.CONCAT($M$3,E14,IF(F14="","","&lt;img src=images\inline\linebrk.png&gt;"),F14,IF(G14="","","&lt;img src=images\inline\linebrk.png&gt;"),G14,IF(H14="","","&lt;img src=images\inline\linebrk.png&gt;"),H14,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Burst Block: &lt;/b&gt;&lt;br&gt;Destroy this card to completely block an incoming attack and deal 5 damage to all adjacent beings.</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="D15" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>119</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="J15" s="7" t="str">
+        <f>IF(D15="yes",_xlfn.CONCAT($N$3,E15,IF(F15="","","&lt;img src=images\inline\linebrk.png&gt;"),F15,IF(G15="","","&lt;img src=images\inline\linebrk.png&gt;"),G15,IF(H15="","","&lt;img src=images\inline\linebrk.png&gt;"),H15,),_xlfn.CONCAT($M$3,E15,IF(F15="","","&lt;img src=images\inline\linebrk.png&gt;"),F15,IF(G15="","","&lt;img src=images\inline\linebrk.png&gt;"),G15,IF(H15="","","&lt;img src=images\inline\linebrk.png&gt;"),H15,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Lay Egg:&lt;/b&gt; 1 AP + (chargeT or  weirdT)&lt;br&gt;Place an explosive egg on an adjacent hex.&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Detonate:&lt;/b&gt; 1 AP&lt;br&gt;All eggs on the map explode, adjacent beings take 5 damage and terrain is destroyed, including walls.</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>11</v>
@@ -1640,20 +1273,20 @@
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="7" t="str">
-        <f>IF(C16="yes",_xlfn.CONCAT($N$3,E16,IF(F16="","","&lt;img src=Images\line.png&gt;"),F16,IF(G16="","","&lt;img src=Images\line.png&gt;"),G16,IF(H16="","","&lt;img src=Images\line.png&gt;"),H16,),_xlfn.CONCAT($M$3,E16,IF(F16="","","&lt;img src=Images\line.png&gt;"),F16,IF(G16="","","&lt;img src=Images\line.png&gt;"),G16,IF(H16="","","&lt;img src=Images\line.png&gt;"),H16,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Crush:&lt;/b&gt; 4 AP or (2 AP + fleshTfleshT)&lt;br&gt;Damage = 8 , close range.&lt;br&gt;Critical Options:&lt;b&gt;&lt;br&gt;Concuss:&lt;/b&gt; Inflict the &lt;b&gt;Stunned&lt;/b&gt; status effect.</v>
+        <f>IF(C16="yes",_xlfn.CONCAT($N$3,E16,IF(F16="","","&lt;img src=images\inline\linebrk.png&gt;"),F16,IF(G16="","","&lt;img src=images\inline\linebrk.png&gt;"),G16,IF(H16="","","&lt;img src=images\inline\linebrk.png&gt;"),H16,),_xlfn.CONCAT($M$3,E16,IF(F16="","","&lt;img src=images\inline\linebrk.png&gt;"),F16,IF(G16="","","&lt;img src=images\inline\linebrk.png&gt;"),G16,IF(H16="","","&lt;img src=images\inline\linebrk.png&gt;"),H16,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Crush:&lt;/b&gt; 4 AP or (2 AP + fleshT fleshT)&lt;br&gt;Damage = 8 , close range.&lt;br&gt;Critical Options:&lt;b&gt;&lt;br&gt;Concuss:&lt;/b&gt; Inflict the &lt;b&gt;Stunned&lt;/b&gt; status effect.</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>11</v>
@@ -1661,61 +1294,66 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="7" t="str">
-        <f>IF(C17="yes",_xlfn.CONCAT($N$3,E17,IF(F17="","","&lt;img src=Images\line.png&gt;"),F17,IF(G17="","","&lt;img src=Images\line.png&gt;"),G17,IF(H17="","","&lt;img src=Images\line.png&gt;"),H17,),_xlfn.CONCAT($M$3,E17,IF(F17="","","&lt;img src=Images\line.png&gt;"),F17,IF(G17="","","&lt;img src=Images\line.png&gt;"),G17,IF(H17="","","&lt;img src=Images\line.png&gt;"),H17,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Bludgeon:&lt;/b&gt; 3 AP&lt;br&gt;Damage = 6 , close range.&lt;img src=Images\line.png&gt;&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Whelm:&lt;/b&gt; 2 AP + weirdT&lt;br&gt;Damage = 3 , close range.&lt;br&gt;Inflicts the &lt;b&gt;Entangled&lt;/b&gt; status effect on a hit.</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <f>IF(C17="yes",_xlfn.CONCAT($N$3,E17,IF(F17="","","&lt;img src=images\inline\linebrk.png&gt;"),F17,IF(G17="","","&lt;img src=images\inline\linebrk.png&gt;"),G17,IF(H17="","","&lt;img src=images\inline\linebrk.png&gt;"),H17,),_xlfn.CONCAT($M$3,E17,IF(F17="","","&lt;img src=images\inline\linebrk.png&gt;"),F17,IF(G17="","","&lt;img src=images\inline\linebrk.png&gt;"),G17,IF(H17="","","&lt;img src=images\inline\linebrk.png&gt;"),H17,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Bludgeon:&lt;/b&gt; 3 AP&lt;br&gt;Damage = 6 , close range.&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Whelm:&lt;/b&gt; 1 AP + weirdT&lt;br&gt;Damage = 3 , close range.&lt;br&gt;Inflicts the &lt;b&gt;Entangled&lt;/b&gt; status effect on a hit.</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="E18" s="8" t="s">
+        <v>122</v>
+      </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
-      <c r="J18" s="10"/>
-    </row>
-    <row r="19" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="J18" s="7" t="str">
+        <f>IF(C18="yes",_xlfn.CONCAT($N$3,E18,IF(F18="","","&lt;img src=images\inline\linebrk.png&gt;"),F18,IF(G18="","","&lt;img src=images\inline\linebrk.png&gt;"),G18,IF(H18="","","&lt;img src=images\inline\linebrk.png&gt;"),H18,),_xlfn.CONCAT($M$3,E18,IF(F18="","","&lt;img src=images\inline\linebrk.png&gt;"),F18,IF(G18="","","&lt;img src=images\inline\linebrk.png&gt;"),G18,IF(H18="","","&lt;img src=images\inline\linebrk.png&gt;"),H18,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Vandalise:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 2 , close range.&lt;br&gt;On a hit, you may destroy this card to destroy any equipped Limb or Impression from the target.</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>52</v>
+      <c r="E19" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="7" t="str">
-        <f>IF(C19="yes",_xlfn.CONCAT($N$3,E19,IF(F19="","","&lt;img src=Images\line.png&gt;"),F19,IF(G19="","","&lt;img src=Images\line.png&gt;"),G19,IF(H19="","","&lt;img src=Images\line.png&gt;"),H19,),_xlfn.CONCAT($M$3,E19,IF(F19="","","&lt;img src=Images\line.png&gt;"),F19,IF(G19="","","&lt;img src=Images\line.png&gt;"),G19,IF(H19="","","&lt;img src=Images\line.png&gt;"),H19,))</f>
-        <v>&lt;p style="font-size:12px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Charge!:&lt;/b&gt; 3 AP or 2 AP +jazzT&lt;br&gt;Damage = hexes moved , close range.&lt;br&gt;You may move any number of hexes in a straight line as part of making the attack. &lt;br&gt;hornshexes&lt;img src=Images\line.png&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Shove :&lt;/b&gt; 1 AP +fleshT&lt;br&gt;Damage = 2 , close range.&lt;br&gt;On a hit, the target is pushed back hexes equal to your &lt;span style="color:#e74c3c"&gt;&lt;strong&gt;Flesh&lt;/strong&gt;&lt;/span&gt;.</v>
+        <f>IF(C19="yes",_xlfn.CONCAT($N$3,E19,IF(F19="","","&lt;img src=images\inline\linebrk.png&gt;"),F19,IF(G19="","","&lt;img src=images\inline\linebrk.png&gt;"),G19,IF(H19="","","&lt;img src=images\inline\linebrk.png&gt;"),H19,),_xlfn.CONCAT($M$3,E19,IF(F19="","","&lt;img src=images\inline\linebrk.png&gt;"),F19,IF(G19="","","&lt;img src=images\inline\linebrk.png&gt;"),G19,IF(H19="","","&lt;img src=images\inline\linebrk.png&gt;"),H19,))</f>
+        <v>&lt;p style="font-size:12px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Charge!:&lt;/b&gt; 2 AP&lt;br&gt;Damage = hexes moved , close range.&lt;br&gt;You may move any number of hexes in a straight line as part of making the attack. &lt;br&gt;hornshexes&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Shove :&lt;/b&gt; 1 AP +fleshT&lt;br&gt;Damage = 2 , close range.&lt;br&gt;On a hit, the target is pushed back hexes equal to your &lt;span style="color:#e74c3c"&gt;&lt;strong&gt;Flesh&lt;/strong&gt;&lt;/span&gt;.</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>11</v>
@@ -1723,22 +1361,20 @@
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>55</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="7" t="str">
-        <f>IF(C20="yes",_xlfn.CONCAT($N$3,E20,IF(F20="","","&lt;img src=Images\line.png&gt;"),F20,IF(G20="","","&lt;img src=Images\line.png&gt;"),G20,IF(H20="","","&lt;img src=Images\line.png&gt;"),H20,),_xlfn.CONCAT($M$3,E20,IF(F20="","","&lt;img src=Images\line.png&gt;"),F20,IF(G20="","","&lt;img src=Images\line.png&gt;"),G20,IF(H20="","","&lt;img src=Images\line.png&gt;"),H20,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Nip:&lt;/b&gt; 2 AP&lt;br&gt;Damage = &lt;span style="color:#e74c3c"&gt;&lt;strong&gt;Flesh&lt;/strong&gt;&lt;/span&gt; , close range.&lt;br&gt;Critical Option:&lt;br&gt;&lt;b&gt;Restrain: &lt;/b&gt;Inflict the &lt;b&gt;Entangled&lt;/b&gt; status effect.&lt;img src=Images\line.png&gt;&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Block: &lt;/b&gt;1 AP&lt;br&gt;Destroy this card to completely block an incoming attack.</v>
+        <f>IF(C20="yes",_xlfn.CONCAT($N$3,E20,IF(F20="","","&lt;img src=images\inline\linebrk.png&gt;"),F20,IF(G20="","","&lt;img src=images\inline\linebrk.png&gt;"),G20,IF(H20="","","&lt;img src=images\inline\linebrk.png&gt;"),H20,),_xlfn.CONCAT($M$3,E20,IF(F20="","","&lt;img src=images\inline\linebrk.png&gt;"),F20,IF(G20="","","&lt;img src=images\inline\linebrk.png&gt;"),G20,IF(H20="","","&lt;img src=images\inline\linebrk.png&gt;"),H20,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Nip:&lt;/b&gt; 2 AP&lt;br&gt;Damage = &lt;span style="color:#e74c3c"&gt;&lt;strong&gt;Flesh&lt;/strong&gt;&lt;/span&gt; , close range.&lt;br&gt;Critical Option:&lt;br&gt;&lt;b&gt;Restrain: &lt;/b&gt;Inflict the &lt;b&gt;Entangled&lt;/b&gt; status effect.</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>11</v>
@@ -1746,22 +1382,22 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="7" t="str">
-        <f>IF(C21="yes",_xlfn.CONCAT($N$3,E21,IF(F21="","","&lt;img src=Images\line.png&gt;"),F21,IF(G21="","","&lt;img src=Images\line.png&gt;"),G21,IF(H21="","","&lt;img src=Images\line.png&gt;"),H21,),_xlfn.CONCAT($M$3,E21,IF(F21="","","&lt;img src=Images\line.png&gt;"),F21,IF(G21="","","&lt;img src=Images\line.png&gt;"),G21,IF(H21="","","&lt;img src=Images\line.png&gt;"),H21,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Bite:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 4 , close range.&lt;br&gt;Critical Option:&lt;br&gt;&lt;b&gt;Exalt:&lt;/b&gt; Restore your composure or gain up to 2 temporary composure.&lt;img src=Images\line.png&gt;&lt;i&gt;Ranged Attack -&lt;/i&gt;&lt;b&gt; Phage: &lt;/b&gt;2 AP&lt;br&gt;Damage = 7 &lt;br&gt;Throw this limb at your target as part of the attack, regardless of attack outcome, they now have Hungering Hand equipped .</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <f>IF(C21="yes",_xlfn.CONCAT($N$3,E21,IF(F21="","","&lt;img src=images\inline\linebrk.png&gt;"),F21,IF(G21="","","&lt;img src=images\inline\linebrk.png&gt;"),G21,IF(H21="","","&lt;img src=images\inline\linebrk.png&gt;"),H21,),_xlfn.CONCAT($M$3,E21,IF(F21="","","&lt;img src=images\inline\linebrk.png&gt;"),F21,IF(G21="","","&lt;img src=images\inline\linebrk.png&gt;"),G21,IF(H21="","","&lt;img src=images\inline\linebrk.png&gt;"),H21,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Bite:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 4 , close range.&lt;br&gt;&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Ranged Attack -&lt;/i&gt;&lt;b&gt; Phage: &lt;/b&gt;2 AP&lt;br&gt;Damage = 7 &lt;br&gt;Throw this limb at your target as part of the attack, regardless of attack outcome, they now have Hungering Hand equipped .</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>11</v>
@@ -1769,49 +1405,47 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>62</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="7" t="str">
-        <f>IF(C22="yes",_xlfn.CONCAT($N$3,E22,IF(F22="","","&lt;img src=Images\line.png&gt;"),F22,IF(G22="","","&lt;img src=Images\line.png&gt;"),G22,IF(H22="","","&lt;img src=Images\line.png&gt;"),H22,),_xlfn.CONCAT($M$3,E22,IF(F22="","","&lt;img src=Images\line.png&gt;"),F22,IF(G22="","","&lt;img src=Images\line.png&gt;"),G22,IF(H22="","","&lt;img src=Images\line.png&gt;"),H22,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Impale: &lt;/b&gt;2 AP&lt;br&gt;Damage = 5 , reach.&lt;br&gt;Must be in lance mode to use.&lt;img src=Images\line.png&gt;&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Iron Petals: &lt;/b&gt;1 AP&lt;br&gt;Destroy this card to completely block an incoming attack.&lt;br&gt;Must be in flower mode to use.&lt;img src=Images\line.png&gt;&lt;b&gt;Bloom/Wither:&lt;/b&gt; 1 AP&lt;br&gt;Switch this card between lance mode or Flower mode. At the start of the combat Lanceflower Bloom begins in Flower mode.</v>
+        <f>IF(C22="yes",_xlfn.CONCAT($N$3,E22,IF(F22="","","&lt;img src=images\inline\linebrk.png&gt;"),F22,IF(G22="","","&lt;img src=images\inline\linebrk.png&gt;"),G22,IF(H22="","","&lt;img src=images\inline\linebrk.png&gt;"),H22,),_xlfn.CONCAT($M$3,E22,IF(F22="","","&lt;img src=images\inline\linebrk.png&gt;"),F22,IF(G22="","","&lt;img src=images\inline\linebrk.png&gt;"),G22,IF(H22="","","&lt;img src=images\inline\linebrk.png&gt;"),H22,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Impale: &lt;/b&gt;2 AP&lt;br&gt;Damage = 4 , reach.&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Bloom: &lt;/b&gt; WeirdT + &lt;b&gt;exhausted&lt;/b&gt; &lt;br&gt;Destroy this card to completely block an incoming attack.</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="7" t="str">
-        <f>IF(C23="yes",_xlfn.CONCAT($N$3,E23,IF(F23="","","&lt;img src=Images\line.png&gt;"),F23,IF(G23="","","&lt;img src=Images\line.png&gt;"),G23,IF(H23="","","&lt;img src=Images\line.png&gt;"),H23,),_xlfn.CONCAT($M$3,E23,IF(F23="","","&lt;img src=Images\line.png&gt;"),F23,IF(G23="","","&lt;img src=Images\line.png&gt;"),G23,IF(H23="","","&lt;img src=Images\line.png&gt;"),H23,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Splinter Trail:&lt;/b&gt; 1 AP + (chargeT or weirdT)&lt;br&gt;For the rest of your turn, leave a conductive trail behind in any hex you move out of.&lt;img src=Images\line.png&gt;&lt;b&gt;Electrify:&lt;/b&gt; 2 AP&lt;br&gt;Electrify an adjacent hex and all connected conductive hexes. All beings electrified take 3 damage. This damage cannot be reduced. Hexes with water are also conductive.</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <f>IF(C23="yes",_xlfn.CONCAT($N$3,E23,IF(F23="","","&lt;img src=images\inline\linebrk.png&gt;"),F23,IF(G23="","","&lt;img src=images\inline\linebrk.png&gt;"),G23,IF(H23="","","&lt;img src=images\inline\linebrk.png&gt;"),H23,),_xlfn.CONCAT($M$3,E23,IF(F23="","","&lt;img src=images\inline\linebrk.png&gt;"),F23,IF(G23="","","&lt;img src=images\inline\linebrk.png&gt;"),G23,IF(H23="","","&lt;img src=images\inline\linebrk.png&gt;"),H23,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Splinter Trail:&lt;/b&gt; 1 AP + (chargeT or weirdT)&lt;br&gt;For the rest of your turn, leave a conductive trail behind in any hex you move out of.&lt;img src=images\inline\linebrk.png&gt;&lt;b&gt;Electrify:&lt;/b&gt; 2 AP&lt;br&gt;Electrify an adjacent hex and all connected conductive hexes. All beings electrified take 3 damage. This damage cannot be reduced. Hexes with water are also conductive.</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>11</v>
@@ -1823,11 +1457,14 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="10"/>
-    </row>
-    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="J24" s="7" t="str">
+        <f>IF(C24="yes",_xlfn.CONCAT($N$3,E24,IF(F24="","","&lt;img src=images\inline\linebrk.png&gt;"),F24,IF(G24="","","&lt;img src=images\inline\linebrk.png&gt;"),G24,IF(H24="","","&lt;img src=images\inline\linebrk.png&gt;"),H24,),_xlfn.CONCAT($M$3,E24,IF(F24="","","&lt;img src=images\inline\linebrk.png&gt;"),F24,IF(G24="","","&lt;img src=images\inline\linebrk.png&gt;"),G24,IF(H24="","","&lt;img src=images\inline\linebrk.png&gt;"),H24,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>11</v>
@@ -1835,22 +1472,22 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="7" t="str">
-        <f>IF(C25="yes",_xlfn.CONCAT($N$3,E25,IF(F25="","","&lt;img src=Images\line.png&gt;"),F25,IF(G25="","","&lt;img src=Images\line.png&gt;"),G25,IF(H25="","","&lt;img src=Images\line.png&gt;"),H25,),_xlfn.CONCAT($M$3,E25,IF(F25="","","&lt;img src=Images\line.png&gt;"),F25,IF(G25="","","&lt;img src=Images\line.png&gt;"),G25,IF(H25="","","&lt;img src=Images\line.png&gt;"),H25,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Gnaw:&lt;/b&gt; 1 AP&lt;br&gt;Damage = 1 , close range.&lt;br&gt;This attack always hits, do not roll.&lt;img src=Images\line.png&gt;il</v>
+        <f>IF(C25="yes",_xlfn.CONCAT($N$3,E25,IF(F25="","","&lt;img src=images\inline\linebrk.png&gt;"),F25,IF(G25="","","&lt;img src=images\inline\linebrk.png&gt;"),G25,IF(H25="","","&lt;img src=images\inline\linebrk.png&gt;"),H25,),_xlfn.CONCAT($M$3,E25,IF(F25="","","&lt;img src=images\inline\linebrk.png&gt;"),F25,IF(G25="","","&lt;img src=images\inline\linebrk.png&gt;"),G25,IF(H25="","","&lt;img src=images\inline\linebrk.png&gt;"),H25,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Gnaw:&lt;/b&gt; 1 AP&lt;br&gt;Damage = 1 , close range.&lt;br&gt;This attack always hits, do not roll.&lt;img src=images\inline\linebrk.png&gt;il</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>11</v>
@@ -1858,22 +1495,22 @@
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="7" t="str">
-        <f>IF(C26="yes",_xlfn.CONCAT($N$3,E26,IF(F26="","","&lt;img src=Images\line.png&gt;"),F26,IF(G26="","","&lt;img src=Images\line.png&gt;"),G26,IF(H26="","","&lt;img src=Images\line.png&gt;"),H26,),_xlfn.CONCAT($M$3,E26,IF(F26="","","&lt;img src=Images\line.png&gt;"),F26,IF(G26="","","&lt;img src=Images\line.png&gt;"),G26,IF(H26="","","&lt;img src=Images\line.png&gt;"),H26,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Nasty Stab:&lt;/b&gt; 3 AP&lt;br&gt;Damage = 6 , close range.&lt;br&gt;Crit options:&lt;br&gt;&lt;b&gt;Armour Piercing:&lt;/b&gt; Ignore damage reduction effects.&lt;br&gt;&lt;b&gt;Strike:&lt;/b&gt; +1 damage.&lt;img src=Images\line.png&gt;&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Lance:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 4 , reach.&lt;br&gt;Crit option:&lt;br&gt;&lt;b&gt;Dash&lt;/b&gt; Take a move action for free.</v>
+        <f>IF(C26="yes",_xlfn.CONCAT($N$3,E26,IF(F26="","","&lt;img src=images\inline\linebrk.png&gt;"),F26,IF(G26="","","&lt;img src=images\inline\linebrk.png&gt;"),G26,IF(H26="","","&lt;img src=images\inline\linebrk.png&gt;"),H26,),_xlfn.CONCAT($M$3,E26,IF(F26="","","&lt;img src=images\inline\linebrk.png&gt;"),F26,IF(G26="","","&lt;img src=images\inline\linebrk.png&gt;"),G26,IF(H26="","","&lt;img src=images\inline\linebrk.png&gt;"),H26,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Nasty Stab:&lt;/b&gt; 3 AP&lt;br&gt;Damage = 6 , close range.&lt;br&gt;Crit options:&lt;br&gt;&lt;b&gt;Armour Piercing:&lt;/b&gt; Ignore damage reduction effects.&lt;br&gt;&lt;b&gt;Strike:&lt;/b&gt; +1 damage.&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Melee Attack - &lt;/i&gt;&lt;b&gt;Lance:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 4 , reach.&lt;br&gt;Crit option:&lt;br&gt;&lt;b&gt;Dash&lt;/b&gt; Take a move action for free.</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>11</v>
@@ -1881,22 +1518,22 @@
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="7" t="str">
-        <f>IF(C27="yes",_xlfn.CONCAT($N$3,E27,IF(F27="","","&lt;img src=Images\line.png&gt;"),F27,IF(G27="","","&lt;img src=Images\line.png&gt;"),G27,IF(H27="","","&lt;img src=Images\line.png&gt;"),H27,),_xlfn.CONCAT($M$3,E27,IF(F27="","","&lt;img src=Images\line.png&gt;"),F27,IF(G27="","","&lt;img src=Images\line.png&gt;"),G27,IF(H27="","","&lt;img src=Images\line.png&gt;"),H27,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Salt in the wound:&lt;/b&gt; 1 AP or weirdT&lt;br&gt;Whenever an adjacent creature takes a wound, you may activate this and inflict the &lt;b&gt;Stunned&lt;/b&gt; status effect on them.&lt;img src=Images\line.png&gt;&lt;i&gt;Passive - &lt;b&gt;Fueled by pain:&lt;/i&gt;&lt;/b&gt;&lt;br&gt;Whenever you take a wound, gain the &lt;b&gt;Well Rested&lt;/b&gt; status effect.</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <f>IF(C27="yes",_xlfn.CONCAT($N$3,E27,IF(F27="","","&lt;img src=images\inline\linebrk.png&gt;"),F27,IF(G27="","","&lt;img src=images\inline\linebrk.png&gt;"),G27,IF(H27="","","&lt;img src=images\inline\linebrk.png&gt;"),H27,),_xlfn.CONCAT($M$3,E27,IF(F27="","","&lt;img src=images\inline\linebrk.png&gt;"),F27,IF(G27="","","&lt;img src=images\inline\linebrk.png&gt;"),G27,IF(H27="","","&lt;img src=images\inline\linebrk.png&gt;"),H27,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Reaction - &lt;/i&gt;&lt;b&gt;Salt in the wound:&lt;/b&gt; 1 AP or weirdT&lt;br&gt;Whenever an adjacent creature takes a wound, you may activate this and inflict the &lt;b&gt;Stunned&lt;/b&gt; status effect on them.&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Passive - &lt;b&gt;Fueled by pain:&lt;/i&gt;&lt;/b&gt;&lt;br&gt;Whenever you take a wound, gain the &lt;b&gt;Well Rested&lt;/b&gt; status effect.</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>11</v>
@@ -1904,22 +1541,22 @@
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="7" t="str">
-        <f>IF(C28="yes",_xlfn.CONCAT($N$3,E28,IF(F28="","","&lt;img src=Images\line.png&gt;"),F28,IF(G28="","","&lt;img src=Images\line.png&gt;"),G28,IF(H28="","","&lt;img src=Images\line.png&gt;"),H28,),_xlfn.CONCAT($M$3,E28,IF(F28="","","&lt;img src=Images\line.png&gt;"),F28,IF(G28="","","&lt;img src=Images\line.png&gt;"),G28,IF(H28="","","&lt;img src=Images\line.png&gt;"),H28,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt; &lt;b&gt;Nip: &lt;/b&gt;2 AP&lt;br&gt;Damage = 3 , close range.&lt;br&gt;Crit option:&lt;br&gt;&lt;b&gt;Strike:&lt;/b&gt; +1 damage.&lt;br&gt;&lt;img src=Images\line.png&gt;&lt;i&gt;Passive - &lt;b&gt; Precise:&lt;/b&gt;&lt;/i&gt;&lt;br&gt;Wounds inflicted by this limb's attacks always target the stat of your choice.</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <f>IF(C28="yes",_xlfn.CONCAT($N$3,E28,IF(F28="","","&lt;img src=images\inline\linebrk.png&gt;"),F28,IF(G28="","","&lt;img src=images\inline\linebrk.png&gt;"),G28,IF(H28="","","&lt;img src=images\inline\linebrk.png&gt;"),H28,),_xlfn.CONCAT($M$3,E28,IF(F28="","","&lt;img src=images\inline\linebrk.png&gt;"),F28,IF(G28="","","&lt;img src=images\inline\linebrk.png&gt;"),G28,IF(H28="","","&lt;img src=images\inline\linebrk.png&gt;"),H28,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt; &lt;b&gt;Nip: &lt;/b&gt;2 AP&lt;br&gt;Damage = 3 , close range.&lt;br&gt;Crit option:&lt;br&gt;&lt;b&gt;Strike:&lt;/b&gt; +1 damage.&lt;br&gt;&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Passive - &lt;b&gt; Precise:&lt;/b&gt;&lt;/i&gt;&lt;br&gt;Wounds inflicted by this limb's attacks always target the stat of your choice.</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>11</v>
@@ -1927,20 +1564,20 @@
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="7" t="str">
-        <f>IF(C29="yes",_xlfn.CONCAT($N$3,E29,IF(F29="","","&lt;img src=Images\line.png&gt;"),F29,IF(G29="","","&lt;img src=Images\line.png&gt;"),G29,IF(H29="","","&lt;img src=Images\line.png&gt;"),H29,),_xlfn.CONCAT($M$3,E29,IF(F29="","","&lt;img src=Images\line.png&gt;"),F29,IF(G29="","","&lt;img src=Images\line.png&gt;"),G29,IF(H29="","","&lt;img src=Images\line.png&gt;"),H29,))</f>
+        <f>IF(C29="yes",_xlfn.CONCAT($N$3,E29,IF(F29="","","&lt;img src=images\inline\linebrk.png&gt;"),F29,IF(G29="","","&lt;img src=images\inline\linebrk.png&gt;"),G29,IF(H29="","","&lt;img src=images\inline\linebrk.png&gt;"),H29,),_xlfn.CONCAT($M$3,E29,IF(F29="","","&lt;img src=images\inline\linebrk.png&gt;"),F29,IF(G29="","","&lt;img src=images\inline\linebrk.png&gt;"),G29,IF(H29="","","&lt;img src=images\inline\linebrk.png&gt;"),H29,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Ranged Attack - &lt;/i&gt;&lt;b&gt;Corrosive spit: &lt;/b&gt;2 AP + weirdT&lt;br&gt;Damage = 4. &lt;br&gt;Ignores damage reduction effects.</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1950,11 +1587,14 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
-      <c r="J30" s="10"/>
-    </row>
-    <row r="31" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="J30" s="7" t="str">
+        <f>IF(C30="yes",_xlfn.CONCAT($N$3,E30,IF(F30="","","&lt;img src=images\inline\linebrk.png&gt;"),F30,IF(G30="","","&lt;img src=images\inline\linebrk.png&gt;"),G30,IF(H30="","","&lt;img src=images\inline\linebrk.png&gt;"),H30,),_xlfn.CONCAT($M$3,E30,IF(F30="","","&lt;img src=images\inline\linebrk.png&gt;"),F30,IF(G30="","","&lt;img src=images\inline\linebrk.png&gt;"),G30,IF(H30="","","&lt;img src=images\inline\linebrk.png&gt;"),H30,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>11</v>
@@ -1962,24 +1602,24 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="7" t="str">
-        <f>IF(C31="yes",_xlfn.CONCAT($N$3,E31,IF(F31="","","&lt;img src=Images\line.png&gt;"),F31,IF(G31="","","&lt;img src=Images\line.png&gt;"),G31,IF(H31="","","&lt;img src=Images\line.png&gt;"),H31,),_xlfn.CONCAT($M$3,E31,IF(F31="","","&lt;img src=Images\line.png&gt;"),F31,IF(G31="","","&lt;img src=Images\line.png&gt;"),G31,IF(H31="","","&lt;img src=Images\line.png&gt;"),H31,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Slam:&lt;/b&gt; 4 AP&lt;br&gt;Damage = 8, close range.&lt;br&gt;&lt;img src=Images\line.png&gt;&lt;b&gt;Wall of Splendor: &lt;/b&gt;1 AP&lt;br&gt;Place the slab down on an adjacent hex, it extends straight on each side to become a three hex wall, if there is space. This wall blocks vision and is indestructable.&lt;img src=Images\line.png&gt;&lt;b&gt;Reclaim: &lt;/b&gt;3 AP or fleshtfleshtfleshT&lt;br&gt;Pick up a deployed painted slab, any adjacent being can do this.</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <f>IF(C31="yes",_xlfn.CONCAT($N$3,E31,IF(F31="","","&lt;img src=images\inline\linebrk.png&gt;"),F31,IF(G31="","","&lt;img src=images\inline\linebrk.png&gt;"),G31,IF(H31="","","&lt;img src=images\inline\linebrk.png&gt;"),H31,),_xlfn.CONCAT($M$3,E31,IF(F31="","","&lt;img src=images\inline\linebrk.png&gt;"),F31,IF(G31="","","&lt;img src=images\inline\linebrk.png&gt;"),G31,IF(H31="","","&lt;img src=images\inline\linebrk.png&gt;"),H31,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Slam:&lt;/b&gt; 4 AP&lt;br&gt;Damage = 8, close range.&lt;br&gt;&lt;img src=images\inline\linebrk.png&gt;&lt;b&gt;Wall of Splendor: &lt;/b&gt;1 AP&lt;br&gt;Place the slab down on an adjacent hex, it extends straight on each side to become a three hex wall, if there is space. This wall blocks vision and is indestructable.&lt;img src=images\inline\linebrk.png&gt;&lt;b&gt;Reclaim: &lt;/b&gt;3 AP or fleshtfleshtfleshT&lt;br&gt;Pick up a deployed painted slab, any adjacent being can do this.</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>11</v>
@@ -1987,20 +1627,20 @@
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="7" t="str">
-        <f>IF(C32="yes",_xlfn.CONCAT($N$3,E32,IF(F32="","","&lt;img src=Images\line.png&gt;"),F32,IF(G32="","","&lt;img src=Images\line.png&gt;"),G32,IF(H32="","","&lt;img src=Images\line.png&gt;"),H32,),_xlfn.CONCAT($M$3,E32,IF(F32="","","&lt;img src=Images\line.png&gt;"),F32,IF(G32="","","&lt;img src=Images\line.png&gt;"),G32,IF(H32="","","&lt;img src=Images\line.png&gt;"),H32,))</f>
+        <f>IF(C32="yes",_xlfn.CONCAT($N$3,E32,IF(F32="","","&lt;img src=images\inline\linebrk.png&gt;"),F32,IF(G32="","","&lt;img src=images\inline\linebrk.png&gt;"),G32,IF(H32="","","&lt;img src=images\inline\linebrk.png&gt;"),H32,),_xlfn.CONCAT($M$3,E32,IF(F32="","","&lt;img src=images\inline\linebrk.png&gt;"),F32,IF(G32="","","&lt;img src=images\inline\linebrk.png&gt;"),G32,IF(H32="","","&lt;img src=images\inline\linebrk.png&gt;"),H32,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Ranged Attack -&lt;/i&gt;&lt;b&gt; Fling:&lt;/b&gt; 2 AP&lt;br&gt;Damage = 4. &lt;br&gt;You take 1 damage when you use this attack.</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>11</v>
@@ -2008,22 +1648,22 @@
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="7" t="str">
-        <f>IF(C33="yes",_xlfn.CONCAT($N$3,E33,IF(F33="","","&lt;img src=Images\line.png&gt;"),F33,IF(G33="","","&lt;img src=Images\line.png&gt;"),G33,IF(H33="","","&lt;img src=Images\line.png&gt;"),H33,),_xlfn.CONCAT($M$3,E33,IF(F33="","","&lt;img src=Images\line.png&gt;"),F33,IF(G33="","","&lt;img src=Images\line.png&gt;"),G33,IF(H33="","","&lt;img src=Images\line.png&gt;"),H33,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Embed:&lt;/b&gt; weirdt&lt;br&gt;Place a 1 hex sized heartstone on an adjacent hex. It will break if it takes damage.&lt;img src=Images\line.png&gt;&lt;i&gt;Passive - &lt;b&gt; Living Rythm:&lt;/i&gt;&lt;/b&gt;&lt;br&gt;While there is at least 1 heartstone on the map, you gain up to 3 temporary composure at the end of your turn.</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <f>IF(C33="yes",_xlfn.CONCAT($N$3,E33,IF(F33="","","&lt;img src=images\inline\linebrk.png&gt;"),F33,IF(G33="","","&lt;img src=images\inline\linebrk.png&gt;"),G33,IF(H33="","","&lt;img src=images\inline\linebrk.png&gt;"),H33,),_xlfn.CONCAT($M$3,E33,IF(F33="","","&lt;img src=images\inline\linebrk.png&gt;"),F33,IF(G33="","","&lt;img src=images\inline\linebrk.png&gt;"),G33,IF(H33="","","&lt;img src=images\inline\linebrk.png&gt;"),H33,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;b&gt;Embed:&lt;/b&gt; weirdt&lt;br&gt;Place a 1 hex sized heartstone on an adjacent hex. It will break if it takes damage.&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Passive - &lt;b&gt; Living Rythm:&lt;/i&gt;&lt;/b&gt;&lt;br&gt;While there is at least 1 heartstone on the map, you gain up to 3 temporary composure at the end of your turn.</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -2033,36 +1673,39 @@
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
-      <c r="J34" s="10"/>
-    </row>
-    <row r="35" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="J34" s="7" t="str">
+        <f>IF(C34="yes",_xlfn.CONCAT($N$3,E34,IF(F34="","","&lt;img src=images\inline\linebrk.png&gt;"),F34,IF(G34="","","&lt;img src=images\inline\linebrk.png&gt;"),G34,IF(H34="","","&lt;img src=images\inline\linebrk.png&gt;"),H34,),_xlfn.CONCAT($M$3,E34,IF(F34="","","&lt;img src=images\inline\linebrk.png&gt;"),F34,IF(G34="","","&lt;img src=images\inline\linebrk.png&gt;"),G34,IF(H34="","","&lt;img src=images\inline\linebrk.png&gt;"),H34,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="7" t="str">
-        <f>IF(C35="yes",_xlfn.CONCAT($N$3,E35,IF(F35="","","&lt;img src=Images\line.png&gt;"),F35,IF(G35="","","&lt;img src=Images\line.png&gt;"),G35,IF(H35="","","&lt;img src=Images\line.png&gt;"),H35,),_xlfn.CONCAT($M$3,E35,IF(F35="","","&lt;img src=Images\line.png&gt;"),F35,IF(G35="","","&lt;img src=Images\line.png&gt;"),G35,IF(H35="","","&lt;img src=Images\line.png&gt;"),H35,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Ranged Attack - &lt;/i&gt;&lt;b&gt;Throw: &lt;/b&gt;1 AP + charget&lt;br&gt;Damage = &lt;span style="color:#e74c3c"&gt;&lt;strong&gt;Flesh&lt;/strong&gt;&lt;/span&gt;.&lt;img src=Images\line.png&gt;&lt;b&gt;Rummage:&lt;/b&gt; 3 AP + fleshT&lt;br&gt;Recharge this item.</v>
+        <f>IF(C35="yes",_xlfn.CONCAT($N$3,E35,IF(F35="","","&lt;img src=images\inline\linebrk.png&gt;"),F35,IF(G35="","","&lt;img src=images\inline\linebrk.png&gt;"),G35,IF(H35="","","&lt;img src=images\inline\linebrk.png&gt;"),H35,),_xlfn.CONCAT($M$3,E35,IF(F35="","","&lt;img src=images\inline\linebrk.png&gt;"),F35,IF(G35="","","&lt;img src=images\inline\linebrk.png&gt;"),G35,IF(H35="","","&lt;img src=images\inline\linebrk.png&gt;"),H35,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Ranged Attack - &lt;/i&gt;&lt;b&gt;Throw: &lt;/b&gt;1 AP + charget&lt;br&gt;Damage = &lt;span style="color:#e74c3c"&gt;&lt;strong&gt;Flesh&lt;/strong&gt;&lt;/span&gt;.&lt;img src=images\inline\linebrk.png&gt;&lt;b&gt;Rummage:&lt;/b&gt; 3 AP + fleshT&lt;br&gt;Recharge this item.</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>11</v>
@@ -2070,22 +1713,22 @@
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="7" t="str">
-        <f>IF(C36="yes",_xlfn.CONCAT($N$3,E36,IF(F36="","","&lt;img src=Images\line.png&gt;"),F36,IF(G36="","","&lt;img src=Images\line.png&gt;"),G36,IF(H36="","","&lt;img src=Images\line.png&gt;"),H36,),_xlfn.CONCAT($M$3,E36,IF(F36="","","&lt;img src=Images\line.png&gt;"),F36,IF(G36="","","&lt;img src=Images\line.png&gt;"),G36,IF(H36="","","&lt;img src=Images\line.png&gt;"),H36,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt; &lt;b&gt;Thump: &lt;/b&gt;2 AP&lt;br&gt;Damage =4, close range.&lt;br&gt;Crit Option:&lt;br&gt;&lt;b&gt;Concuss:&lt;/b&gt; Inflict the &lt;b&gt;Stunned&lt;/b&gt; status effect.&lt;img src=Images\line.png&gt;&lt;b&gt;Dig:&lt;/b&gt; 1 AP or fleshT&lt;br&gt;Clear an adjacent hex of any player generated terrain features.</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <f>IF(C36="yes",_xlfn.CONCAT($N$3,E36,IF(F36="","","&lt;img src=images\inline\linebrk.png&gt;"),F36,IF(G36="","","&lt;img src=images\inline\linebrk.png&gt;"),G36,IF(H36="","","&lt;img src=images\inline\linebrk.png&gt;"),H36,),_xlfn.CONCAT($M$3,E36,IF(F36="","","&lt;img src=images\inline\linebrk.png&gt;"),F36,IF(G36="","","&lt;img src=images\inline\linebrk.png&gt;"),G36,IF(H36="","","&lt;img src=images\inline\linebrk.png&gt;"),H36,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt; &lt;b&gt;Thump: &lt;/b&gt;2 AP&lt;br&gt;Damage =4, close range.&lt;br&gt;Crit Option:&lt;br&gt;&lt;b&gt;Concuss:&lt;/b&gt; Inflict the &lt;b&gt;Stunned&lt;/b&gt; status effect.&lt;img src=images\inline\linebrk.png&gt;&lt;b&gt;Dig:&lt;/b&gt; 1 AP or fleshT&lt;br&gt;Clear an adjacent hex of any player generated terrain features.</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>11</v>
@@ -2093,20 +1736,20 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
       <c r="J37" s="7" t="str">
-        <f>_xlfn.CONCAT(M$3,E37,IF(F37="","","&lt;img src=Images\line.png&gt;"),F37,IF(G37="","","&lt;img src=Images\line.png&gt;"),G37,IF(H37="","","&lt;img src=Images\line.png&gt;"),H37,)</f>
+        <f>IF(C37="yes",_xlfn.CONCAT($N$3,E37,IF(F37="","","&lt;img src=images\inline\linebrk.png&gt;"),F37,IF(G37="","","&lt;img src=images\inline\linebrk.png&gt;"),G37,IF(H37="","","&lt;img src=images\inline\linebrk.png&gt;"),H37,),_xlfn.CONCAT($M$3,E37,IF(F37="","","&lt;img src=images\inline\linebrk.png&gt;"),F37,IF(G37="","","&lt;img src=images\inline\linebrk.png&gt;"),G37,IF(H37="","","&lt;img src=images\inline\linebrk.png&gt;"),H37,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Ranged Attack&lt;/i&gt; -&lt;b&gt; Yoink:&lt;/b&gt; 1 AP&lt;br&gt;Damage = 0.&lt;br&gt;Pull the target to an adjacent hex on a hit&lt;br&gt;Crit Option:&lt;br&gt;&lt;b&gt;Entangle:&lt;/b&gt; Inflict the &lt;b&gt;Entangled&lt;/b&gt; status effect.</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>11</v>
@@ -2114,22 +1757,22 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
       <c r="J38" s="7" t="str">
-        <f>IF(C38="yes",_xlfn.CONCAT($N$3,E38,IF(F38="","","&lt;img src=Images\line.png&gt;"),F38,IF(G38="","","&lt;img src=Images\line.png&gt;"),G38,IF(H38="","","&lt;img src=Images\line.png&gt;"),H38,),_xlfn.CONCAT($M$3,E38,IF(F38="","","&lt;img src=Images\line.png&gt;"),F38,IF(G38="","","&lt;img src=Images\line.png&gt;"),G38,IF(H38="","","&lt;img src=Images\line.png&gt;"),H38,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Slime Glob: &lt;/b&gt;2 AP&lt;br&gt;Damage = 2, reach.&lt;br&gt;Inflicts the &lt;b&gt;Entangled&lt;/b&gt; status effect on a hit.&lt;img src=Images\line.png&gt;&lt;i&gt;Passive - &lt;b&gt; Secretions:&lt;/i&gt;&lt;/b&gt;&lt;br&gt;When you take a move action, you may spend weirdt to leave a trail of goo in all hexes moved out of. Moving through this goo costs 2 hexes of movement per hex.</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <f>IF(C38="yes",_xlfn.CONCAT($N$3,E38,IF(F38="","","&lt;img src=images\inline\linebrk.png&gt;"),F38,IF(G38="","","&lt;img src=images\inline\linebrk.png&gt;"),G38,IF(H38="","","&lt;img src=images\inline\linebrk.png&gt;"),H38,),_xlfn.CONCAT($M$3,E38,IF(F38="","","&lt;img src=images\inline\linebrk.png&gt;"),F38,IF(G38="","","&lt;img src=images\inline\linebrk.png&gt;"),G38,IF(H38="","","&lt;img src=images\inline\linebrk.png&gt;"),H38,))</f>
+        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;&lt;i&gt;Melee Attack -&lt;/i&gt;&lt;b&gt; Slime Glob: &lt;/b&gt;2 AP&lt;br&gt;Damage = 2, reach.&lt;br&gt;Inflicts the &lt;b&gt;Entangled&lt;/b&gt; status effect on a hit.&lt;img src=images\inline\linebrk.png&gt;&lt;i&gt;Passive - &lt;b&gt; Secretions:&lt;/i&gt;&lt;/b&gt;&lt;br&gt;When you take a move action, you may spend weirdt to leave a trail of goo in all hexes moved out of. Moving through this goo costs 2 hexes of movement per hex.</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>11</v>
@@ -2142,13 +1785,13 @@
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
       <c r="J39" s="7" t="str">
-        <f>IF(C39="yes",_xlfn.CONCAT($N$3,E39,IF(F39="","","&lt;img src=Images\line.png&gt;"),F39,IF(G39="","","&lt;img src=Images\line.png&gt;"),G39,IF(H39="","","&lt;img src=Images\line.png&gt;"),H39,),_xlfn.CONCAT($M$3,E39,IF(F39="","","&lt;img src=Images\line.png&gt;"),F39,IF(G39="","","&lt;img src=Images\line.png&gt;"),G39,IF(H39="","","&lt;img src=Images\line.png&gt;"),H39,))</f>
+        <f>IF(C39="yes",_xlfn.CONCAT($N$3,E39,IF(F39="","","&lt;img src=images\inline\linebrk.png&gt;"),F39,IF(G39="","","&lt;img src=images\inline\linebrk.png&gt;"),G39,IF(H39="","","&lt;img src=images\inline\linebrk.png&gt;"),H39,),_xlfn.CONCAT($M$3,E39,IF(F39="","","&lt;img src=images\inline\linebrk.png&gt;"),F39,IF(G39="","","&lt;img src=images\inline\linebrk.png&gt;"),G39,IF(H39="","","&lt;img src=images\inline\linebrk.png&gt;"),H39,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>11</v>
@@ -2161,13 +1804,13 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="7" t="str">
-        <f>IF(C40="yes",_xlfn.CONCAT($N$3,E40,IF(F40="","","&lt;img src=Images\line.png&gt;"),F40,IF(G40="","","&lt;img src=Images\line.png&gt;"),G40,IF(H40="","","&lt;img src=Images\line.png&gt;"),H40,),_xlfn.CONCAT($M$3,E40,IF(F40="","","&lt;img src=Images\line.png&gt;"),F40,IF(G40="","","&lt;img src=Images\line.png&gt;"),G40,IF(H40="","","&lt;img src=Images\line.png&gt;"),H40,))</f>
+        <f>IF(C40="yes",_xlfn.CONCAT($N$3,E40,IF(F40="","","&lt;img src=images\inline\linebrk.png&gt;"),F40,IF(G40="","","&lt;img src=images\inline\linebrk.png&gt;"),G40,IF(H40="","","&lt;img src=images\inline\linebrk.png&gt;"),H40,),_xlfn.CONCAT($M$3,E40,IF(F40="","","&lt;img src=images\inline\linebrk.png&gt;"),F40,IF(G40="","","&lt;img src=images\inline\linebrk.png&gt;"),G40,IF(H40="","","&lt;img src=images\inline\linebrk.png&gt;"),H40,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>11</v>
@@ -2180,13 +1823,13 @@
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
       <c r="J41" s="7" t="str">
-        <f>IF(C41="yes",_xlfn.CONCAT($N$3,E41,IF(F41="","","&lt;img src=Images\line.png&gt;"),F41,IF(G41="","","&lt;img src=Images\line.png&gt;"),G41,IF(H41="","","&lt;img src=Images\line.png&gt;"),H41,),_xlfn.CONCAT($M$3,E41,IF(F41="","","&lt;img src=Images\line.png&gt;"),F41,IF(G41="","","&lt;img src=Images\line.png&gt;"),G41,IF(H41="","","&lt;img src=Images\line.png&gt;"),H41,))</f>
+        <f>IF(C41="yes",_xlfn.CONCAT($N$3,E41,IF(F41="","","&lt;img src=images\inline\linebrk.png&gt;"),F41,IF(G41="","","&lt;img src=images\inline\linebrk.png&gt;"),G41,IF(H41="","","&lt;img src=images\inline\linebrk.png&gt;"),H41,),_xlfn.CONCAT($M$3,E41,IF(F41="","","&lt;img src=images\inline\linebrk.png&gt;"),F41,IF(G41="","","&lt;img src=images\inline\linebrk.png&gt;"),G41,IF(H41="","","&lt;img src=images\inline\linebrk.png&gt;"),H41,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>11</v>
@@ -2199,13 +1842,13 @@
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="J42" s="7" t="str">
-        <f>IF(C42="yes",_xlfn.CONCAT($N$3,E42,IF(F42="","","&lt;img src=Images\line.png&gt;"),F42,IF(G42="","","&lt;img src=Images\line.png&gt;"),G42,IF(H42="","","&lt;img src=Images\line.png&gt;"),H42,),_xlfn.CONCAT($M$3,E42,IF(F42="","","&lt;img src=Images\line.png&gt;"),F42,IF(G42="","","&lt;img src=Images\line.png&gt;"),G42,IF(H42="","","&lt;img src=Images\line.png&gt;"),H42,))</f>
+        <f>IF(C42="yes",_xlfn.CONCAT($N$3,E42,IF(F42="","","&lt;img src=images\inline\linebrk.png&gt;"),F42,IF(G42="","","&lt;img src=images\inline\linebrk.png&gt;"),G42,IF(H42="","","&lt;img src=images\inline\linebrk.png&gt;"),H42,),_xlfn.CONCAT($M$3,E42,IF(F42="","","&lt;img src=images\inline\linebrk.png&gt;"),F42,IF(G42="","","&lt;img src=images\inline\linebrk.png&gt;"),G42,IF(H42="","","&lt;img src=images\inline\linebrk.png&gt;"),H42,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>11</v>
@@ -2218,13 +1861,13 @@
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="J43" s="7" t="str">
-        <f>IF(C43="yes",_xlfn.CONCAT($N$3,E43,IF(F43="","","&lt;img src=Images\line.png&gt;"),F43,IF(G43="","","&lt;img src=Images\line.png&gt;"),G43,IF(H43="","","&lt;img src=Images\line.png&gt;"),H43,),_xlfn.CONCAT($M$3,E43,IF(F43="","","&lt;img src=Images\line.png&gt;"),F43,IF(G43="","","&lt;img src=Images\line.png&gt;"),G43,IF(H43="","","&lt;img src=Images\line.png&gt;"),H43,))</f>
+        <f>IF(C43="yes",_xlfn.CONCAT($N$3,E43,IF(F43="","","&lt;img src=images\inline\linebrk.png&gt;"),F43,IF(G43="","","&lt;img src=images\inline\linebrk.png&gt;"),G43,IF(H43="","","&lt;img src=images\inline\linebrk.png&gt;"),H43,),_xlfn.CONCAT($M$3,E43,IF(F43="","","&lt;img src=images\inline\linebrk.png&gt;"),F43,IF(G43="","","&lt;img src=images\inline\linebrk.png&gt;"),G43,IF(H43="","","&lt;img src=images\inline\linebrk.png&gt;"),H43,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>11</v>
@@ -2237,13 +1880,13 @@
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="7" t="str">
-        <f>IF(C44="yes",_xlfn.CONCAT($N$3,E44,IF(F44="","","&lt;img src=Images\line.png&gt;"),F44,IF(G44="","","&lt;img src=Images\line.png&gt;"),G44,IF(H44="","","&lt;img src=Images\line.png&gt;"),H44,),_xlfn.CONCAT($M$3,E44,IF(F44="","","&lt;img src=Images\line.png&gt;"),F44,IF(G44="","","&lt;img src=Images\line.png&gt;"),G44,IF(H44="","","&lt;img src=Images\line.png&gt;"),H44,))</f>
+        <f>IF(C44="yes",_xlfn.CONCAT($N$3,E44,IF(F44="","","&lt;img src=images\inline\linebrk.png&gt;"),F44,IF(G44="","","&lt;img src=images\inline\linebrk.png&gt;"),G44,IF(H44="","","&lt;img src=images\inline\linebrk.png&gt;"),H44,),_xlfn.CONCAT($M$3,E44,IF(F44="","","&lt;img src=images\inline\linebrk.png&gt;"),F44,IF(G44="","","&lt;img src=images\inline\linebrk.png&gt;"),G44,IF(H44="","","&lt;img src=images\inline\linebrk.png&gt;"),H44,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>11</v>
@@ -2256,13 +1899,13 @@
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="7" t="str">
-        <f>IF(C45="yes",_xlfn.CONCAT($N$3,E45,IF(F45="","","&lt;img src=Images\line.png&gt;"),F45,IF(G45="","","&lt;img src=Images\line.png&gt;"),G45,IF(H45="","","&lt;img src=Images\line.png&gt;"),H45,),_xlfn.CONCAT($M$3,E45,IF(F45="","","&lt;img src=Images\line.png&gt;"),F45,IF(G45="","","&lt;img src=Images\line.png&gt;"),G45,IF(H45="","","&lt;img src=Images\line.png&gt;"),H45,))</f>
+        <f>IF(C45="yes",_xlfn.CONCAT($N$3,E45,IF(F45="","","&lt;img src=images\inline\linebrk.png&gt;"),F45,IF(G45="","","&lt;img src=images\inline\linebrk.png&gt;"),G45,IF(H45="","","&lt;img src=images\inline\linebrk.png&gt;"),H45,),_xlfn.CONCAT($M$3,E45,IF(F45="","","&lt;img src=images\inline\linebrk.png&gt;"),F45,IF(G45="","","&lt;img src=images\inline\linebrk.png&gt;"),G45,IF(H45="","","&lt;img src=images\inline\linebrk.png&gt;"),H45,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>11</v>
@@ -2275,13 +1918,13 @@
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="7" t="str">
-        <f>IF(C46="yes",_xlfn.CONCAT($N$3,E46,IF(F46="","","&lt;img src=Images\line.png&gt;"),F46,IF(G46="","","&lt;img src=Images\line.png&gt;"),G46,IF(H46="","","&lt;img src=Images\line.png&gt;"),H46,),_xlfn.CONCAT($M$3,E46,IF(F46="","","&lt;img src=Images\line.png&gt;"),F46,IF(G46="","","&lt;img src=Images\line.png&gt;"),G46,IF(H46="","","&lt;img src=Images\line.png&gt;"),H46,))</f>
+        <f>IF(C46="yes",_xlfn.CONCAT($N$3,E46,IF(F46="","","&lt;img src=images\inline\linebrk.png&gt;"),F46,IF(G46="","","&lt;img src=images\inline\linebrk.png&gt;"),G46,IF(H46="","","&lt;img src=images\inline\linebrk.png&gt;"),H46,),_xlfn.CONCAT($M$3,E46,IF(F46="","","&lt;img src=images\inline\linebrk.png&gt;"),F46,IF(G46="","","&lt;img src=images\inline\linebrk.png&gt;"),G46,IF(H46="","","&lt;img src=images\inline\linebrk.png&gt;"),H46,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>11</v>
@@ -2294,13 +1937,13 @@
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
       <c r="J47" s="7" t="str">
-        <f>IF(C47="yes",_xlfn.CONCAT($N$3,E47,IF(F47="","","&lt;img src=Images\line.png&gt;"),F47,IF(G47="","","&lt;img src=Images\line.png&gt;"),G47,IF(H47="","","&lt;img src=Images\line.png&gt;"),H47,),_xlfn.CONCAT($M$3,E47,IF(F47="","","&lt;img src=Images\line.png&gt;"),F47,IF(G47="","","&lt;img src=Images\line.png&gt;"),G47,IF(H47="","","&lt;img src=Images\line.png&gt;"),H47,))</f>
+        <f>IF(C47="yes",_xlfn.CONCAT($N$3,E47,IF(F47="","","&lt;img src=images\inline\linebrk.png&gt;"),F47,IF(G47="","","&lt;img src=images\inline\linebrk.png&gt;"),G47,IF(H47="","","&lt;img src=images\inline\linebrk.png&gt;"),H47,),_xlfn.CONCAT($M$3,E47,IF(F47="","","&lt;img src=images\inline\linebrk.png&gt;"),F47,IF(G47="","","&lt;img src=images\inline\linebrk.png&gt;"),G47,IF(H47="","","&lt;img src=images\inline\linebrk.png&gt;"),H47,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>11</v>
@@ -2313,13 +1956,13 @@
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
       <c r="J48" s="7" t="str">
-        <f>IF(C48="yes",_xlfn.CONCAT($N$3,E48,IF(F48="","","&lt;img src=Images\line.png&gt;"),F48,IF(G48="","","&lt;img src=Images\line.png&gt;"),G48,IF(H48="","","&lt;img src=Images\line.png&gt;"),H48,),_xlfn.CONCAT($M$3,E48,IF(F48="","","&lt;img src=Images\line.png&gt;"),F48,IF(G48="","","&lt;img src=Images\line.png&gt;"),G48,IF(H48="","","&lt;img src=Images\line.png&gt;"),H48,))</f>
+        <f>IF(C48="yes",_xlfn.CONCAT($N$3,E48,IF(F48="","","&lt;img src=images\inline\linebrk.png&gt;"),F48,IF(G48="","","&lt;img src=images\inline\linebrk.png&gt;"),G48,IF(H48="","","&lt;img src=images\inline\linebrk.png&gt;"),H48,),_xlfn.CONCAT($M$3,E48,IF(F48="","","&lt;img src=images\inline\linebrk.png&gt;"),F48,IF(G48="","","&lt;img src=images\inline\linebrk.png&gt;"),G48,IF(H48="","","&lt;img src=images\inline\linebrk.png&gt;"),H48,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>11</v>
@@ -2332,13 +1975,13 @@
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
       <c r="J49" s="7" t="str">
-        <f>IF(C49="yes",_xlfn.CONCAT($N$3,E49,IF(F49="","","&lt;img src=Images\line.png&gt;"),F49,IF(G49="","","&lt;img src=Images\line.png&gt;"),G49,IF(H49="","","&lt;img src=Images\line.png&gt;"),H49,),_xlfn.CONCAT($M$3,E49,IF(F49="","","&lt;img src=Images\line.png&gt;"),F49,IF(G49="","","&lt;img src=Images\line.png&gt;"),G49,IF(H49="","","&lt;img src=Images\line.png&gt;"),H49,))</f>
+        <f>IF(C49="yes",_xlfn.CONCAT($N$3,E49,IF(F49="","","&lt;img src=images\inline\linebrk.png&gt;"),F49,IF(G49="","","&lt;img src=images\inline\linebrk.png&gt;"),G49,IF(H49="","","&lt;img src=images\inline\linebrk.png&gt;"),H49,),_xlfn.CONCAT($M$3,E49,IF(F49="","","&lt;img src=images\inline\linebrk.png&gt;"),F49,IF(G49="","","&lt;img src=images\inline\linebrk.png&gt;"),G49,IF(H49="","","&lt;img src=images\inline\linebrk.png&gt;"),H49,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>11</v>
@@ -2351,7 +1994,7 @@
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="J50" s="7" t="str">
-        <f>IF(C50="yes",_xlfn.CONCAT($N$3,E50,IF(F50="","","&lt;img src=Images\line.png&gt;"),F50,IF(G50="","","&lt;img src=Images\line.png&gt;"),G50,IF(H50="","","&lt;img src=Images\line.png&gt;"),H50,),_xlfn.CONCAT($M$3,E50,IF(F50="","","&lt;img src=Images\line.png&gt;"),F50,IF(G50="","","&lt;img src=Images\line.png&gt;"),G50,IF(H50="","","&lt;img src=Images\line.png&gt;"),H50,))</f>
+        <f>IF(C50="yes",_xlfn.CONCAT($N$3,E50,IF(F50="","","&lt;img src=images\inline\linebrk.png&gt;"),F50,IF(G50="","","&lt;img src=images\inline\linebrk.png&gt;"),G50,IF(H50="","","&lt;img src=images\inline\linebrk.png&gt;"),H50,),_xlfn.CONCAT($M$3,E50,IF(F50="","","&lt;img src=images\inline\linebrk.png&gt;"),F50,IF(G50="","","&lt;img src=images\inline\linebrk.png&gt;"),G50,IF(H50="","","&lt;img src=images\inline\linebrk.png&gt;"),H50,))</f>
         <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
       </c>
     </row>
@@ -2365,10 +2008,7 @@
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
-      <c r="J51" s="7" t="str">
-        <f>IF(C51="yes",_xlfn.CONCAT($N$3,E51,IF(F51="","","&lt;img src=Images\line.png&gt;"),F51,IF(G51="","","&lt;img src=Images\line.png&gt;"),G51,IF(H51="","","&lt;img src=Images\line.png&gt;"),H51,),_xlfn.CONCAT($M$3,E51,IF(F51="","","&lt;img src=Images\line.png&gt;"),F51,IF(G51="","","&lt;img src=Images\line.png&gt;"),G51,IF(H51="","","&lt;img src=Images\line.png&gt;"),H51,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
-      </c>
+      <c r="J51" s="7"/>
     </row>
     <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
@@ -2380,10 +2020,7 @@
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
-      <c r="J52" s="7" t="str">
-        <f>IF(C52="yes",_xlfn.CONCAT($N$3,E52,IF(F52="","","&lt;img src=Images\line.png&gt;"),F52,IF(G52="","","&lt;img src=Images\line.png&gt;"),G52,IF(H52="","","&lt;img src=Images\line.png&gt;"),H52,),_xlfn.CONCAT($M$3,E52,IF(F52="","","&lt;img src=Images\line.png&gt;"),F52,IF(G52="","","&lt;img src=Images\line.png&gt;"),G52,IF(H52="","","&lt;img src=Images\line.png&gt;"),H52,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
-      </c>
+      <c r="J52" s="7"/>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
@@ -2395,10 +2032,7 @@
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
-      <c r="J53" s="7" t="str">
-        <f>IF(C53="yes",_xlfn.CONCAT($N$3,E53,IF(F53="","","&lt;img src=Images\line.png&gt;"),F53,IF(G53="","","&lt;img src=Images\line.png&gt;"),G53,IF(H53="","","&lt;img src=Images\line.png&gt;"),H53,),_xlfn.CONCAT($M$3,E53,IF(F53="","","&lt;img src=Images\line.png&gt;"),F53,IF(G53="","","&lt;img src=Images\line.png&gt;"),G53,IF(H53="","","&lt;img src=Images\line.png&gt;"),H53,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
-      </c>
+      <c r="J53" s="7"/>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
@@ -2410,68 +2044,25 @@
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
-      <c r="J54" s="7" t="str">
-        <f>IF(C54="yes",_xlfn.CONCAT($N$3,E54,IF(F54="","","&lt;img src=Images\line.png&gt;"),F54,IF(G54="","","&lt;img src=Images\line.png&gt;"),G54,IF(H54="","","&lt;img src=Images\line.png&gt;"),H54,),_xlfn.CONCAT($M$3,E54,IF(F54="","","&lt;img src=Images\line.png&gt;"),F54,IF(G54="","","&lt;img src=Images\line.png&gt;"),G54,IF(H54="","","&lt;img src=Images\line.png&gt;"),H54,))</f>
-        <v>&lt;p style="font-size:14px;"&gt;&lt;br&gt;</v>
-      </c>
+      <c r="J54" s="7"/>
     </row>
     <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>116</v>
-      </c>
+      <c r="A63" s="9"/>
     </row>
     <row r="66" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>117</v>
-      </c>
+      <c r="A66" s="9"/>
     </row>
     <row r="68" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>119</v>
-      </c>
+      <c r="A68" s="9"/>
     </row>
     <row r="71" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
-        <v>105</v>
-      </c>
+      <c r="A71" s="9"/>
     </row>
     <row r="72" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>120</v>
-      </c>
+      <c r="A72" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:C54">
+  <conditionalFormatting sqref="B1:C14 B16:C54 B15 D15">
     <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Accessory">
       <formula>NOT(ISERROR(SEARCH("Accessory",B1)))</formula>
     </cfRule>

</xml_diff>